<commit_message>
Add inventory value report.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi_1.xlsx
+++ b/test/integration/project/data_laba_rugi_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="18" activeTab="24"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="16" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="fakturbeli" sheetId="61" r:id="rId1"/>
@@ -33,12 +33,15 @@
     <sheet name="penyesuaianstok" sheetId="84" r:id="rId24"/>
     <sheet name="penyesuaianstok_items" sheetId="85" r:id="rId25"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="145">
   <si>
     <t>id</t>
   </si>
@@ -2903,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7000</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>700</v>
@@ -2924,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3057,6 +3060,9 @@
       <c r="S2">
         <v>1</v>
       </c>
+      <c r="T2">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -3101,6 +3107,9 @@
       <c r="S3">
         <v>1</v>
       </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3144,6 +3153,9 @@
       </c>
       <c r="S4">
         <v>1</v>
+      </c>
+      <c r="T4">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3496,10 +3508,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3585,6 +3597,57 @@
       </c>
       <c r="E4">
         <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41976</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41976</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
+        <v>41976</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes can't display all purchase invoices.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi_1.xlsx
+++ b/test/integration/project/data_laba_rugi_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="16" activeTab="24"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fakturbeli" sheetId="61" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="144">
   <si>
     <t>id</t>
   </si>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>FakturJual_id</t>
-  </si>
-  <si>
-    <t>gudang</t>
   </si>
   <si>
     <t>sequence_name</t>
@@ -863,7 +860,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1012,7 +1009,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="F1:F1048576 D1:D1048576"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1063,10 +1060,10 @@
         <v>28</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1074,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1">
         <v>41976</v>
@@ -1089,7 +1086,7 @@
         <v>5</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1103,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1">
         <v>41988</v>
@@ -1118,7 +1115,7 @@
         <v>5</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -1132,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="1">
         <v>41992</v>
@@ -1147,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -1177,7 +1174,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -1186,7 +1183,7 @@
         <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1241,7 +1238,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" activeCellId="2" sqref="D1:D1048576 J1 J1:J1048576"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1276,16 +1273,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>10</v>
@@ -1311,16 +1308,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
         <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>112</v>
       </c>
       <c r="D2" s="1">
         <v>41976</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
@@ -1332,7 +1329,7 @@
         <v>5</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1340,16 +1337,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="1">
         <v>41998</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
@@ -1361,7 +1358,7 @@
         <v>5</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1369,16 +1366,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1">
         <v>42000</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
@@ -1390,7 +1387,7 @@
         <v>5</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1411,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -1423,7 +1420,7 @@
         <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1648,16 +1645,16 @@
         <v>700</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
         <v>116</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>117</v>
-      </c>
-      <c r="J2" t="s">
-        <v>118</v>
       </c>
       <c r="K2" s="1">
         <v>41974</v>
@@ -1674,25 +1671,25 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" t="s">
         <v>119</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>120</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" t="s">
         <v>121</v>
-      </c>
-      <c r="I3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" t="s">
-        <v>122</v>
       </c>
       <c r="K3" s="1">
         <v>41976</v>
@@ -1712,22 +1709,22 @@
         <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" t="s">
         <v>123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>124</v>
       </c>
       <c r="H4" t="s">
         <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K4" s="1">
         <v>41981</v>
@@ -1744,25 +1741,25 @@
         <v>600</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" t="s">
         <v>125</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>126</v>
       </c>
-      <c r="H5" t="s">
-        <v>127</v>
-      </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K5" s="1">
         <v>41988</v>
@@ -1779,25 +1776,25 @@
         <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" t="s">
         <v>128</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>129</v>
       </c>
-      <c r="H6" t="s">
-        <v>130</v>
-      </c>
       <c r="I6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K6" s="1">
         <v>41992</v>
@@ -1817,22 +1814,22 @@
         <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" t="s">
         <v>131</v>
-      </c>
-      <c r="G7" t="s">
-        <v>132</v>
       </c>
       <c r="H7" t="s">
         <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K7" s="1">
         <v>41998</v>
@@ -1852,22 +1849,22 @@
         <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" t="s">
         <v>133</v>
-      </c>
-      <c r="G8" t="s">
-        <v>134</v>
       </c>
       <c r="H8" t="s">
         <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K8" s="1">
         <v>42000</v>
@@ -1886,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2006,7 +2003,7 @@
         <v>41976</v>
       </c>
       <c r="O2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -2086,7 +2083,7 @@
         <v>57</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>22</v>
@@ -2097,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="1">
         <v>41976</v>
@@ -2132,7 +2129,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" s="1">
         <v>41988</v>
@@ -2167,7 +2164,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F4" s="1">
         <v>41992</v>
@@ -2222,7 +2219,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>46</v>
@@ -2345,7 +2342,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2362,7 +2359,7 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2475,7 +2472,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2506,7 +2503,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
@@ -2538,13 +2535,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s">
         <v>141</v>
       </c>
-      <c r="H2" t="s">
-        <v>142</v>
-      </c>
       <c r="J2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2628,7 +2625,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2696,7 +2693,7 @@
         <v>41976</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2771,7 +2768,7 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2784,7 +2781,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2806,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>10</v>
@@ -2853,13 +2850,13 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J2" s="1">
         <v>41974</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2871,7 +2868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2886,7 +2883,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>54</v>
@@ -2898,7 +2895,7 @@
         <v>29</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2927,7 +2924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
@@ -3267,8 +3264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3314,7 +3311,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -3326,7 +3323,7 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -3351,15 +3348,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3367,7 +3364,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3375,7 +3372,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3391,7 +3388,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3399,7 +3396,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3407,7 +3404,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3415,7 +3412,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3423,7 +3420,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3431,7 +3428,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3439,7 +3436,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3447,7 +3444,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3455,7 +3452,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3463,7 +3460,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3471,7 +3468,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3479,7 +3476,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3487,7 +3484,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3495,7 +3492,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3675,19 +3672,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -3696,7 +3693,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3709,7 +3706,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" activeCellId="1" sqref="D1:D1048576 I1:I1048576"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3744,10 +3741,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -3765,13 +3762,13 @@
         <v>27</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -3800,7 +3797,7 @@
         <v>41976.859756944446</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L2">
         <v>0</v>

</xml_diff>

<commit_message>
Permanently store calculated balance in database.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi_1.xlsx
+++ b/test/integration/project/data_laba_rugi_1.xlsx
@@ -1680,7 +1680,7 @@
         <v>100</v>
       </c>
       <c r="C3" s="6">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="E3" t="s">
         <v>81</v>
@@ -1718,7 +1718,7 @@
         <v>-500</v>
       </c>
       <c r="C4" s="6">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -1756,7 +1756,7 @@
         <v>600</v>
       </c>
       <c r="C5" s="6">
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="E5" t="s">
         <v>81</v>
@@ -1794,7 +1794,7 @@
         <v>200</v>
       </c>
       <c r="C6" s="6">
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="E6" t="s">
         <v>81</v>
@@ -1832,7 +1832,7 @@
         <v>-400</v>
       </c>
       <c r="C7" s="6">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E7" t="s">
         <v>63</v>
@@ -1870,7 +1870,7 @@
         <v>-100</v>
       </c>
       <c r="C8" s="6">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="E8" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Change income statements calculation.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi_1.xlsx
+++ b/test/integration/project/data_laba_rugi_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="24" activeTab="30"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="18" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="fakturbeli" sheetId="61" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="161">
   <si>
     <t>id</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t>000013-RS-KB-122014</t>
+  </si>
+  <si>
+    <t>labaRugi</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1639,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2706,7 +2709,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3003,10 +3006,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3022,7 +3025,7 @@
     <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3050,8 +3053,11 @@
       <c r="I1" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -3076,8 +3082,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-1</v>
       </c>
@@ -3098,6 +3107,9 @@
       </c>
       <c r="I3">
         <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3759,7 +3771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add more detail to income statements.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi_1.xlsx
+++ b/test/integration/project/data_laba_rugi_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="18" activeTab="25"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="fakturbeli" sheetId="61" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="165">
   <si>
     <t>id</t>
   </si>
@@ -530,6 +530,18 @@
   </si>
   <si>
     <t>labaRugi</t>
+  </si>
+  <si>
+    <t>FakturJualEceran</t>
+  </si>
+  <si>
+    <t>000001/122014/ECERAN</t>
+  </si>
+  <si>
+    <t>eceran</t>
+  </si>
+  <si>
+    <t>000004-SJ-KB-122014</t>
   </si>
 </sst>
 </file>
@@ -579,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -587,6 +599,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1449,6 +1464,32 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41977</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1">
+        <v>41976</v>
+      </c>
+      <c r="K5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1456,9 +1497,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1521,6 +1564,20 @@
         <v>1</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
     </row>
@@ -3008,7 +3065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -3480,10 +3537,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3493,7 +3550,7 @@
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
@@ -3711,6 +3768,38 @@
       </c>
       <c r="T4">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="1">
+        <v>41982</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1">
+        <v>41982</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3850,9 +3939,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3940,6 +4031,23 @@
         <v>1</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
     </row>

</xml_diff>